<commit_message>
Perform dbcan/cayman substrate comparisons and enrichment at different substrate levels in CRC context
</commit_message>
<xml_diff>
--- a/data/Glycan_Annotations/20250219_Table_S1_incl_dbCAN3_annotations.xlsx
+++ b/data/Glycan_Annotations/20250219_Table_S1_incl_dbCAN3_annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Users\Ducarmon_Quinten\EMBL\cayman_paper\data\Glycan_Annotations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDFF7CF-F5C4-473B-B7E2-8793353B93AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012ACC75-61D7-40E0-8793-5D1B0FD30723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1380" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4371,9 +4371,6 @@
     <t>homogalacturonan,rhamnogalacturonan,human_milk_glycan,mucin_glycan</t>
   </si>
   <si>
-    <t>Pectin,Glycoproteins</t>
-  </si>
-  <si>
     <t>Mannans_and_Heteromannans,Glycoprotein</t>
   </si>
   <si>
@@ -4900,6 +4897,9 @@
   </si>
   <si>
     <t>GT111</t>
+  </si>
+  <si>
+    <t>Pectin,Glycoprotein</t>
   </si>
 </sst>
 </file>
@@ -4995,10 +4995,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5290,8 +5286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N672"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6606,7 +6602,7 @@
         <v>120</v>
       </c>
       <c r="E32" t="s">
-        <v>1445</v>
+        <v>1621</v>
       </c>
       <c r="F32" t="s">
         <v>122</v>
@@ -6814,7 +6810,7 @@
         <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F37" t="s">
         <v>136</v>
@@ -6884,7 +6880,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -7171,7 +7167,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>37</v>
@@ -7195,7 +7191,7 @@
         <v>168</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="J46" t="s">
         <v>20</v>
@@ -7309,7 +7305,7 @@
         <v>179</v>
       </c>
       <c r="E49" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="F49" t="s">
         <v>180</v>
@@ -7350,7 +7346,7 @@
         <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F50" t="s">
         <v>185</v>
@@ -7971,7 +7967,7 @@
         <v>15</v>
       </c>
       <c r="E65" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F65" t="s">
         <v>231</v>
@@ -8176,7 +8172,7 @@
         <v>249</v>
       </c>
       <c r="E70" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F70" t="s">
         <v>250</v>
@@ -8188,7 +8184,7 @@
         <v>251</v>
       </c>
       <c r="I70" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="J70" t="s">
         <v>20</v>
@@ -9014,7 +9010,7 @@
         <v>794</v>
       </c>
       <c r="E90" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="F90" t="s">
         <v>322</v>
@@ -9582,7 +9578,7 @@
         <v>15</v>
       </c>
       <c r="E107" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F107" t="s">
         <v>326</v>
@@ -12599,7 +12595,7 @@
         <v>315</v>
       </c>
       <c r="C198" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="D198" t="s">
         <v>120</v>
@@ -12617,7 +12613,7 @@
         <v>550</v>
       </c>
       <c r="I198" s="4" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="J198" t="s">
         <v>20</v>
@@ -12873,7 +12869,7 @@
         <v>15</v>
       </c>
       <c r="E206" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F206" t="s">
         <v>549</v>
@@ -13551,13 +13547,13 @@
         <v>119</v>
       </c>
       <c r="C227" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D227" t="s">
         <v>616</v>
       </c>
       <c r="E227" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="F227" t="s">
         <v>617</v>
@@ -13595,10 +13591,10 @@
         <v>178</v>
       </c>
       <c r="D228" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E228" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="F228" t="s">
         <v>622</v>
@@ -13642,7 +13638,7 @@
         <v>249</v>
       </c>
       <c r="E229" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F229" t="s">
         <v>625</v>
@@ -13721,10 +13717,10 @@
         <v>178</v>
       </c>
       <c r="D231" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E231" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="F231" t="s">
         <v>633</v>
@@ -13894,7 +13890,7 @@
         <v>120</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="F235" t="s">
         <v>642</v>
@@ -13906,7 +13902,7 @@
         <v>643</v>
       </c>
       <c r="I235" s="4" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="J235" t="s">
         <v>20</v>
@@ -13979,7 +13975,7 @@
         <v>249</v>
       </c>
       <c r="E237" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F237" t="s">
         <v>649</v>
@@ -14352,7 +14348,7 @@
         <v>794</v>
       </c>
       <c r="E248" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="F248" t="s">
         <v>677</v>
@@ -14396,7 +14392,7 @@
         <v>15</v>
       </c>
       <c r="E249" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F249" t="s">
         <v>681</v>
@@ -14437,7 +14433,7 @@
         <v>249</v>
       </c>
       <c r="E250" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F250" t="s">
         <v>684</v>
@@ -14481,7 +14477,7 @@
         <v>37</v>
       </c>
       <c r="E251" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F251" t="s">
         <v>688</v>
@@ -14522,7 +14518,7 @@
         <v>15</v>
       </c>
       <c r="E252" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="F252" t="s">
         <v>692</v>
@@ -14534,7 +14530,7 @@
         <v>693</v>
       </c>
       <c r="I252" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="J252" t="s">
         <v>20</v>
@@ -14566,7 +14562,7 @@
         <v>120</v>
       </c>
       <c r="E253" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="F253" t="s">
         <v>696</v>
@@ -14578,7 +14574,7 @@
         <v>697</v>
       </c>
       <c r="I253" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="J253" t="s">
         <v>20</v>
@@ -14736,7 +14732,7 @@
         <v>120</v>
       </c>
       <c r="E257" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="F257" t="s">
         <v>715</v>
@@ -16222,7 +16218,7 @@
         <v>15</v>
       </c>
       <c r="E301" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F301" t="s">
         <v>795</v>
@@ -16234,7 +16230,7 @@
         <v>796</v>
       </c>
       <c r="I301" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J301" t="s">
         <v>20</v>
@@ -16606,7 +16602,7 @@
         <v>37</v>
       </c>
       <c r="E310" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F310" t="s">
         <v>830</v>
@@ -16647,7 +16643,7 @@
         <v>37</v>
       </c>
       <c r="E311" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F311" t="s">
         <v>832</v>
@@ -16937,7 +16933,7 @@
         <v>15</v>
       </c>
       <c r="E318" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F318" t="s">
         <v>857</v>
@@ -17116,7 +17112,7 @@
         <v>869</v>
       </c>
       <c r="I322" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="J322" t="s">
         <v>20</v>
@@ -17526,7 +17522,7 @@
         <v>37</v>
       </c>
       <c r="E332" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F332" t="s">
         <v>900</v>
@@ -17567,7 +17563,7 @@
         <v>37</v>
       </c>
       <c r="E333" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F333" t="s">
         <v>904</v>
@@ -17608,7 +17604,7 @@
         <v>37</v>
       </c>
       <c r="E334" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F334" t="s">
         <v>908</v>
@@ -17775,7 +17771,7 @@
         <v>37</v>
       </c>
       <c r="E338" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F338" t="s">
         <v>922</v>
@@ -17860,7 +17856,7 @@
         <v>15</v>
       </c>
       <c r="E340" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F340" t="s">
         <v>929</v>
@@ -17901,7 +17897,7 @@
         <v>15</v>
       </c>
       <c r="E341" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F341" t="s">
         <v>932</v>
@@ -18027,7 +18023,7 @@
         <v>249</v>
       </c>
       <c r="E344" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F344" t="s">
         <v>944</v>
@@ -18112,7 +18108,7 @@
         <v>950</v>
       </c>
       <c r="E346" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="F346" t="s">
         <v>951</v>
@@ -18124,7 +18120,7 @@
         <v>952</v>
       </c>
       <c r="I346" s="4" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="J346" t="s">
         <v>20</v>
@@ -18200,7 +18196,7 @@
         <v>15</v>
       </c>
       <c r="E348" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F348" t="s">
         <v>959</v>
@@ -18282,7 +18278,7 @@
         <v>37</v>
       </c>
       <c r="E350" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F350" t="s">
         <v>965</v>
@@ -18616,7 +18612,7 @@
         <v>37</v>
       </c>
       <c r="E358" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F358" t="s">
         <v>985</v>
@@ -18657,7 +18653,7 @@
         <v>120</v>
       </c>
       <c r="E359" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="F359" t="s">
         <v>988</v>
@@ -18669,7 +18665,7 @@
         <v>989</v>
       </c>
       <c r="I359" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="J359" t="s">
         <v>20</v>
@@ -18742,7 +18738,7 @@
         <v>249</v>
       </c>
       <c r="E361" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F361" t="s">
         <v>995</v>
@@ -19205,7 +19201,7 @@
         <v>37</v>
       </c>
       <c r="E372" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F372" t="s">
         <v>1028</v>
@@ -19460,7 +19456,7 @@
         <v>37</v>
       </c>
       <c r="E378" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F378" t="s">
         <v>1046</v>
@@ -19504,7 +19500,7 @@
         <v>15</v>
       </c>
       <c r="E379" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F379" t="s">
         <v>1050</v>
@@ -19762,7 +19758,7 @@
         <v>249</v>
       </c>
       <c r="E385" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F385" t="s">
         <v>1067</v>
@@ -19774,7 +19770,7 @@
         <v>1068</v>
       </c>
       <c r="I385" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="J385" t="s">
         <v>20</v>
@@ -20386,7 +20382,7 @@
         <v>249</v>
       </c>
       <c r="E400" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F400" t="s">
         <v>1104</v>
@@ -20398,7 +20394,7 @@
         <v>1105</v>
       </c>
       <c r="I400" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="J400" t="s">
         <v>20</v>
@@ -20556,7 +20552,7 @@
         <v>37</v>
       </c>
       <c r="E404" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F404" t="s">
         <v>1116</v>
@@ -21183,7 +21179,7 @@
         <v>15</v>
       </c>
       <c r="E419" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F419" t="s">
         <v>1151</v>
@@ -24930,1170 +24926,1170 @@
     </row>
     <row r="527" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F527" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="G527" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="528" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F528" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="G528" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="529" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F529" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="G529" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="530" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F530" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G530" t="s">
         <v>1478</v>
-      </c>
-      <c r="G530" t="s">
-        <v>1479</v>
       </c>
     </row>
     <row r="531" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F531" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="G531" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="532" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F532" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="G532" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="533" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F533" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="G533" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="534" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F534" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G534" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="535" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F535" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="G535" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="536" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F536" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="G536" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="537" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F537" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G537" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="538" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F538" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="G538" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="539" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F539" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="G539" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="540" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F540" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="G540" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="541" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F541" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="G541" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="542" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F542" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="G542" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="543" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F543" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="G543" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="544" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F544" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="G544" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="545" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F545" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="G545" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="546" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F546" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="G546" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="547" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F547" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="G547" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="548" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F548" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="G548" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="549" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F549" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="G549" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="550" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F550" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="G550" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="551" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F551" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="G551" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="552" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F552" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="G552" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="553" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F553" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="G553" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="554" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F554" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="G554" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="555" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F555" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="G555" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="556" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F556" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G556" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="557" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F557" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G557" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="558" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F558" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="G558" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="559" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F559" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="G559" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="560" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F560" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="G560" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="561" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F561" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="G561" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="562" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F562" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="G562" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="563" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F563" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G563" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="564" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F564" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="G564" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="565" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F565" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="G565" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="566" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F566" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="G566" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="567" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F567" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="G567" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="568" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F568" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="G568" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="569" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F569" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="G569" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="570" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F570" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="G570" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="571" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F571" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="G571" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="572" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F572" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="G572" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="573" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F573" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="G573" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="574" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F574" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="G574" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="575" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F575" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="G575" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="576" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F576" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="G576" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="577" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F577" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="G577" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="578" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F578" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="G578" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="579" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F579" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="G579" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="580" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F580" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="G580" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="581" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F581" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="G581" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="582" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F582" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="G582" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="583" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F583" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="G583" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="584" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F584" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="G584" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="585" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F585" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="G585" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="586" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F586" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="G586" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="587" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F587" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="G587" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="588" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F588" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="G588" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="589" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F589" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="G589" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="590" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F590" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="G590" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="591" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F591" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G591" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="592" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F592" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="G592" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="593" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F593" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="G593" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="594" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F594" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="G594" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="595" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F595" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="G595" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="596" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F596" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="G596" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="597" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F597" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G597" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="598" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F598" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="G598" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="599" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F599" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="G599" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="600" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F600" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="G600" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="601" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F601" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G601" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="602" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F602" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="G602" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="603" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F603" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="G603" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="604" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F604" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="G604" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="605" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F605" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="G605" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="606" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F606" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="G606" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="607" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F607" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="G607" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="608" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F608" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="G608" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="609" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F609" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="G609" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="610" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F610" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="G610" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="611" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F611" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="G611" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="612" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F612" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="G612" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="613" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F613" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="G613" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="614" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F614" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="G614" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="615" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F615" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="G615" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="616" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F616" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="G616" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="617" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F617" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="G617" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="618" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F618" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="G618" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="619" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F619" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="G619" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="620" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F620" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="G620" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="621" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F621" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="G621" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="622" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F622" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="G622" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="623" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F623" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="G623" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="624" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F624" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="G624" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="625" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F625" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="G625" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="626" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F626" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="G626" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="627" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F627" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="G627" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="628" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F628" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="G628" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="629" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F629" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="G629" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="630" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F630" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="G630" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="631" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F631" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="G631" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="632" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F632" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="G632" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="633" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F633" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="G633" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="634" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F634" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="G634" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="635" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F635" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="G635" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="636" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F636" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="G636" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="637" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F637" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="G637" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="638" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F638" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="G638" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="639" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F639" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="G639" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="640" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F640" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="G640" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="641" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F641" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="G641" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="642" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F642" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="G642" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="643" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F643" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="G643" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="644" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F644" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="G644" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="645" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F645" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="G645" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="646" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F646" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="G646" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="647" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F647" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="G647" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="648" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F648" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="G648" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="649" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F649" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="G649" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="650" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F650" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="G650" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="651" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F651" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="G651" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="652" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F652" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="G652" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="653" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F653" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="G653" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="654" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F654" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="G654" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="655" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F655" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="G655" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="656" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F656" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="G656" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="657" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F657" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="G657" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="658" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F658" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="G658" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="659" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F659" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="G659" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="660" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F660" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="G660" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="661" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F661" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="G661" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="662" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F662" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="G662" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="663" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F663" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G663" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="664" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F664" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="G664" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="665" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F665" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="G665" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="666" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F666" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="G666" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="667" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F667" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="G667" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="668" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F668" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="G668" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="669" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F669" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="G669" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="670" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F670" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="G670" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="671" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F671" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="G671" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="672" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F672" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="G672" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>